<commit_message>
changed timepoint to integer type in variable_capacity_factors.tab
</commit_message>
<xml_diff>
--- a/R/20190218_FCe_Switch_Inputs.xlsx
+++ b/R/20190218_FCe_Switch_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trins/GoogleDrive/1UT/0_Research/3_Switch/Test_Model/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFB2E3A-3D4B-A948-AF3C-7B8A0A154172}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456947FF-1594-704A-B134-4448037384AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="5" activeTab="11" xr2:uid="{6C4ED1B5-7714-8147-9F70-EE425DA1B5C1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="5" activeTab="8" xr2:uid="{6C4ED1B5-7714-8147-9F70-EE425DA1B5C1}"/>
   </bookViews>
   <sheets>
     <sheet name="periods.tab" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="gen_build_costs.tab" sheetId="12" r:id="rId11"/>
     <sheet name="variable_capacity_factors.tab" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029" calcCompleted="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -11843,7 +11843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC06462-0637-6A4F-943B-9D4F9CE1E2A2}">
   <dimension ref="A1:C795"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -21231,11 +21231,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CDFB17-C25D-F74B-A73A-062E66D727FF}">
   <dimension ref="A1:J398"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>